<commit_message>
* AverageLogger 테스트 추가
</commit_message>
<xml_diff>
--- a/ReleaseChecklist.xlsx
+++ b/ReleaseChecklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="11490" windowHeight="5565"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="11496" windowHeight="5568"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,12 +535,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <selection pane="topRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -817,7 +817,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -830,7 +830,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* reintroduce 최대한 제거
</commit_message>
<xml_diff>
--- a/ReleaseChecklist.xlsx
+++ b/ReleaseChecklist.xlsx
@@ -18,10 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
-    <t>GlobalSettings의 버전 수정</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Version.nsh 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -123,6 +119,10 @@
   </si>
   <si>
     <t>중지</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VersionPublisher의 버전 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -535,7 +535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H12" sqref="H12"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999"/>
@@ -545,52 +545,52 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -599,12 +599,12 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -613,7 +613,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
@@ -625,12 +625,12 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -639,7 +639,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -651,7 +651,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -663,7 +663,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -675,12 +675,12 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -689,12 +689,12 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -703,7 +703,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5">
         <v>42140.479571759257</v>
@@ -722,12 +722,12 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
         <v>42140.483043981483</v>
@@ -736,7 +736,7 @@
         <v>42141.522666435187</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5">
         <v>42149.448279745367</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -759,12 +759,12 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -772,12 +772,12 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5">
         <v>42140.486485995367</v>

</xml_diff>

<commit_message>
* Commit completed release checklist
</commit_message>
<xml_diff>
--- a/ReleaseChecklist.xlsx
+++ b/ReleaseChecklist.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnivProject\SSDTools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11496" windowHeight="5568"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Version.nsh 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -123,14 +128,18 @@
   </si>
   <si>
     <t>VersionPublisher의 버전 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.0.9</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +252,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -289,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,9 +338,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,20 +549,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -568,8 +587,11 @@
       <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -582,8 +604,9 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -596,8 +619,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -610,8 +634,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -622,8 +647,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,8 +662,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -648,8 +675,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -660,8 +688,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -672,8 +701,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -686,8 +716,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -700,8 +731,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -724,8 +756,11 @@
       <c r="H12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="5">
+        <v>42358.649265277774</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -745,8 +780,9 @@
         <v>42190.352436921297</v>
       </c>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -756,8 +792,9 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -769,8 +806,9 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -783,7 +821,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -803,6 +841,9 @@
         <v>42190.357494212964</v>
       </c>
       <c r="G17" s="2"/>
+      <c r="I17" s="5">
+        <v>42358.667345023146</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -812,12 +853,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -825,12 +866,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Added NVMe plugin setup build file * Released 5.1.0
</commit_message>
<xml_diff>
--- a/ReleaseChecklist.xlsx
+++ b/ReleaseChecklist.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Version.nsh 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -132,13 +132,17 @@
   </si>
   <si>
     <t>5.0.9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -550,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I17" sqref="I17"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -562,7 +566,7 @@
     <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -590,8 +594,11 @@
       <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -605,8 +612,9 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -620,8 +628,9 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,8 +644,9 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -648,8 +658,9 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +674,9 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,8 +688,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -689,8 +702,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -702,8 +716,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,8 +732,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,8 +748,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -759,8 +776,9 @@
       <c r="I12" s="5">
         <v>42358.649265277774</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -781,8 +799,9 @@
       </c>
       <c r="G13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -793,8 +812,9 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -807,8 +827,9 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -820,8 +841,9 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -843,6 +865,9 @@
       <c r="G17" s="2"/>
       <c r="I17" s="5">
         <v>42358.667345023146</v>
+      </c>
+      <c r="J17" s="5">
+        <v>42364.648486458333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* SM951 <=> PM951 문제 해결
</commit_message>
<xml_diff>
--- a/ReleaseChecklist.xlsx
+++ b/ReleaseChecklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Version.nsh 수정</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -176,6 +176,10 @@
   </si>
   <si>
     <t>5.2.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2.2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -628,11 +632,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U10" sqref="U10"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -640,7 +644,7 @@
     <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -704,8 +708,11 @@
       <c r="U1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -731,8 +738,9 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -758,8 +766,9 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -785,8 +794,9 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -810,8 +820,9 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,8 +848,9 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -862,8 +874,9 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -887,8 +900,9 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -914,8 +928,9 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,7 +957,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -965,8 +980,9 @@
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1019,9 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,8 +1043,9 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1050,8 +1068,10 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1073,8 +1093,10 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1125,6 +1147,8 @@
       <c r="S16" s="5">
         <v>42420.648666782407</v>
       </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>